<commit_message>
i forgot to update the mapping spreadsheet to reflect the new disposition codes.  This commit addresses that.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/ojbc/OJBC_Disposition_Codes.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Disposition_Reporting_Service/artifacts/service_model/information_model/Disposition_Report_IEPD/documentation/ojbc/OJBC_Disposition_Codes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="15" windowWidth="19425" windowHeight="13065" tabRatio="771"/>
+    <workbookView xWindow="3580" yWindow="20" windowWidth="19420" windowHeight="13060" tabRatio="771"/>
   </bookViews>
   <sheets>
     <sheet name="CourtDisp" sheetId="12" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>OTHER</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Missing/Unknown</t>
   </si>
@@ -36,82 +33,40 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CONV</t>
-  </si>
-  <si>
     <t>Convicted</t>
   </si>
   <si>
-    <t>ACQ</t>
-  </si>
-  <si>
     <t>Acquitted</t>
   </si>
   <si>
     <t>Dismissed</t>
   </si>
   <si>
-    <t>DIS</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
     <t>Civil Procedure</t>
   </si>
   <si>
     <t>Off Calendar</t>
   </si>
   <si>
-    <t>OC</t>
-  </si>
-  <si>
-    <t>NGRI</t>
-  </si>
-  <si>
-    <t>GBMI</t>
-  </si>
-  <si>
     <t>Guilty But Mentally Ill</t>
   </si>
   <si>
     <t>Probation Without Verdict</t>
   </si>
   <si>
-    <t>TTJC</t>
-  </si>
-  <si>
     <t>Transferred to Juvenile Court</t>
   </si>
   <si>
     <t>Mistrial</t>
   </si>
   <si>
-    <t>MIST</t>
-  </si>
-  <si>
     <t>Nolle Prosequi</t>
   </si>
   <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>EXTR</t>
-  </si>
-  <si>
     <t>Extradited</t>
   </si>
   <si>
-    <t>NDBC</t>
-  </si>
-  <si>
     <t>Not Disposition By Court</t>
-  </si>
-  <si>
-    <t>MU</t>
-  </si>
-  <si>
-    <t>PWOV</t>
   </si>
   <si>
     <t>Not Guilty by Reason of Insanity</t>
@@ -197,48 +152,50 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -290,7 +247,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -298,6 +255,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -305,6 +263,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,156 +566,156 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="15">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="15">
       <c r="A2" s="10" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="12">
       <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="C3" s="5"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -765,7 +724,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>